<commit_message>
Sync Pack Qty between GL and Data
</commit_message>
<xml_diff>
--- a/data/suppliers.xlsx
+++ b/data/suppliers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willjackson/Library/CloudStorage/GoogleDrive-wj@wovenandwoods.com/Shared drives/Office/Product Data/Rakata Import Tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/willjackson/Library/CloudStorage/GoogleDrive-wj@wovenandwoods.com/Shared drives/Office/Product Data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2856CB-8577-A741-9746-242729067FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1B7B5C-2F35-AA4A-96A9-E562ED7301CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" xr2:uid="{2FF9D3EE-C52E-4540-953E-4AB69AC2E4E8}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="420">
   <si>
     <t>Name</t>
   </si>
@@ -1281,6 +1281,25 @@
   </si>
   <si>
     <t>SP4 7LN</t>
+  </si>
+  <si>
+    <t>Flooring Sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+01372 232 060</t>
+  </si>
+  <si>
+    <t>https://www.flooringsales.co.uk</t>
+  </si>
+  <si>
+    <t>Unit A Blenheim Trade Centre, Blenheim Road</t>
+  </si>
+  <si>
+    <t>Epsom</t>
+  </si>
+  <si>
+    <t>KT19 9XX</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1353,19 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFF2CC"/>
+          <bgColor rgb="FFFFF2CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1664,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F830770-B2B0-D547-B68A-51C1DD58AC7D}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:K52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="G52" sqref="G52"/>
+    <sheetView tabSelected="1" topLeftCell="E46" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3017,140 +3048,122 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>74</v>
-      </c>
       <c r="B39" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>59</v>
+        <v>406</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>97</v>
+        <v>407</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>142</v>
+        <v>408</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>190</v>
+        <v>409</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>232</v>
+        <v>410</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>273</v>
+        <v>411</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>306</v>
+        <v>412</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>341</v>
+        <v>413</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>75</v>
-      </c>
       <c r="B40" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>100</v>
+        <v>391</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>400</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>193</v>
+        <v>401</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>402</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>214</v>
+        <v>403</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>252</v>
+        <v>404</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>319</v>
+        <v>405</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="1">
-        <v>165</v>
-      </c>
       <c r="B41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>82</v>
+        <v>390</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>393</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>175</v>
+        <v>394</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>392</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>250</v>
+        <v>396</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>290</v>
+        <v>397</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>327</v>
+        <v>398</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>359</v>
+        <v>399</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>123</v>
+        <v>74</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>378</v>
+        <v>232</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>263</v>
+        <v>273</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>380</v>
+        <v>306</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>331</v>
+        <v>341</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>359</v>
@@ -3158,34 +3171,34 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>359</v>
@@ -3193,34 +3206,34 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>77</v>
+        <v>165</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>228</v>
+        <v>377</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>359</v>
@@ -3228,34 +3241,34 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>160</v>
+        <v>123</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>245</v>
+        <v>378</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>290</v>
+        <v>380</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>354</v>
+        <v>331</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>359</v>
@@ -3263,34 +3276,34 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="K46" s="1" t="s">
         <v>359</v>
@@ -3298,34 +3311,34 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>359</v>
@@ -3333,140 +3346,190 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
+        <v>160</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>79</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>8</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>80</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B51" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C51" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D48" s="1" t="s">
+      <c r="D51" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F51" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G51" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H51" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="I48" s="1" t="s">
+      <c r="I51" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="J48" s="1" t="s">
+      <c r="J51" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="K48" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B49" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="D49" s="2" t="s">
+      <c r="K51" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="E49" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>392</v>
-      </c>
-      <c r="G49" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="H49" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="J49" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="J50" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="K50" s="1" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="K51" s="1" t="s">
+      <c r="E52" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>419</v>
+      </c>
+      <c r="K52" s="1" t="s">
         <v>359</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:K48" xr:uid="{0F830770-B2B0-D547-B68A-51C1DD58AC7D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K49">
-      <sortCondition ref="B1:B49"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K51">
+      <sortCondition ref="B1:B51"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
     <hyperlink ref="D38" r:id="rId1" xr:uid="{5FB62680-2219-AA46-9F3E-22C23B94F4D0}"/>
     <hyperlink ref="D33" r:id="rId2" xr:uid="{32702874-3D97-DA46-AE5A-744EAB7BFD05}"/>
     <hyperlink ref="D18" r:id="rId3" xr:uid="{F298995C-7C09-9442-835E-E55B2683A05B}"/>
-    <hyperlink ref="F49" r:id="rId4" xr:uid="{221AB3BF-AF67-C94D-B7C1-659BAE3548A1}"/>
-    <hyperlink ref="D49" r:id="rId5" xr:uid="{9D725C5A-AEF6-3246-9231-2968EA2F1A93}"/>
-    <hyperlink ref="D50" r:id="rId6" xr:uid="{BB5AABD5-7DB0-E844-B287-7416C119F3FE}"/>
-    <hyperlink ref="F50" r:id="rId7" xr:uid="{DE5E8F48-59AC-0E48-9CBC-28AAD38B785F}"/>
+    <hyperlink ref="F41" r:id="rId4" xr:uid="{221AB3BF-AF67-C94D-B7C1-659BAE3548A1}"/>
+    <hyperlink ref="D41" r:id="rId5" xr:uid="{9D725C5A-AEF6-3246-9231-2968EA2F1A93}"/>
+    <hyperlink ref="D40" r:id="rId6" xr:uid="{BB5AABD5-7DB0-E844-B287-7416C119F3FE}"/>
+    <hyperlink ref="F40" r:id="rId7" xr:uid="{DE5E8F48-59AC-0E48-9CBC-28AAD38B785F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>